<commit_message>
sửa lại để có thể lấy tổng số case bị fail, kể cả ignore
</commit_message>
<xml_diff>
--- a/ExcelFile/ChannelTestCase.xlsx
+++ b/ExcelFile/ChannelTestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QC fresher\Automation\Exercise2\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BFE5FB-A9D6-427E-9D5D-2368A12AB840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA3FD8B-46E1-452F-BD2D-9D4D8C46F7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A88D4D40-DE2A-4B7B-92FB-FD6D793C9607}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A88D4D40-DE2A-4B7B-92FB-FD6D793C9607}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="47">
   <si>
     <t>Test case</t>
   </si>
@@ -119,12 +119,6 @@
     <t>TC5</t>
   </si>
   <si>
-    <t>TC6</t>
-  </si>
-  <si>
-    <t>TC7</t>
-  </si>
-  <si>
     <t>CheatID</t>
   </si>
   <si>
@@ -183,6 +177,9 @@
   </si>
   <si>
     <t>64</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -607,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00FF45F-0E6A-4B83-BE00-0F6DFB90CB65}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,22 +671,6 @@
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +708,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -743,7 +724,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -762,10 +743,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -847,13 +828,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -891,7 +872,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -907,10 +888,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -929,7 +910,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -948,7 +929,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -961,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>20</v>
@@ -1004,7 +985,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1020,7 +1001,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -1039,10 +1020,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1124,13 +1105,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1168,7 +1149,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -1200,7 +1181,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>20</v>
@@ -1247,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1263,7 +1244,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -1282,10 +1263,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1367,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1411,7 +1392,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -1443,7 +1424,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>20</v>
@@ -1466,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEAB140-46BE-4F76-849B-EBF08A0BD99A}">
   <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1471,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1506,7 +1487,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -1514,7 +1495,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C4" s="14"/>
     </row>
@@ -1525,10 +1506,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1610,13 +1591,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1654,7 +1635,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -1686,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>20</v>
@@ -1733,7 +1714,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1749,7 +1730,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -1768,10 +1749,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1853,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1897,7 +1878,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -1913,10 +1894,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1935,7 +1916,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -1954,7 +1935,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -1967,7 +1948,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>20</v>

</xml_diff>